<commit_message>
roundController Data To Client
</commit_message>
<xml_diff>
--- a/excels/difficulty.xlsx
+++ b/excels/difficulty.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>难度配置</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>difficulty_local_CN_2</t>
+  </si>
+  <si>
+    <t>difficulty_local_CN_3</t>
+  </si>
+  <si>
+    <t>difficulty_local_CN_4</t>
+  </si>
+  <si>
+    <t>difficulty_local_CN_5</t>
   </si>
 </sst>
 </file>
@@ -980,16 +989,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="3" width="21.1818181818182" customWidth="1"/>
+    <col min="2" max="2" width="32.0909090909091" customWidth="1"/>
+    <col min="3" max="3" width="21.1818181818182" customWidth="1"/>
+    <col min="4" max="4" width="27.3636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1037,6 +1048,48 @@
       </c>
       <c r="D4">
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>